<commit_message>
test the troncated pipeline
</commit_message>
<xml_diff>
--- a/vmdefs.xlsx
+++ b/vmdefs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\My Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF215DF-4B39-49F1-8045-EF8AFED7CEF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9F480C-66CE-4C13-8232-BDA37195305F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{34D50B9A-C40D-4772-AE96-867572325A1F}"/>
   </bookViews>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="317">
   <si>
     <t>DOMAIN</t>
   </si>
@@ -1012,21 +1012,6 @@
   </si>
   <si>
     <t>VM TEST LNX</t>
-  </si>
-  <si>
-    <t>VSL-POC-AIA-001</t>
-  </si>
-  <si>
-    <t>AIA POC LNX</t>
-  </si>
-  <si>
-    <t>vsl-poc-aia-001</t>
-  </si>
-  <si>
-    <t>192.168.25.106</t>
-  </si>
-  <si>
-    <t>192.168.25.1</t>
   </si>
   <si>
     <t>lu717</t>
@@ -1430,10 +1415,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91DAEDD9-6941-4909-B148-BE39F1BC44CD}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:U49"/>
+  <dimension ref="A1:U48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1551,14 +1536,14 @@
         <v>21</v>
       </c>
       <c r="I2" s="2" t="str">
-        <f t="shared" ref="I2:I31" si="0">"sub_"&amp;G2</f>
+        <f t="shared" ref="I2:I30" si="0">"sub_"&amp;G2</f>
         <v>sub_cluster651</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>214</v>
       </c>
       <c r="K2" s="3" t="str">
-        <f t="shared" ref="K2:K48" si="1">"stg_"&amp;G2</f>
+        <f t="shared" ref="K2:K47" si="1">"stg_"&amp;G2</f>
         <v>stg_cluster651</v>
       </c>
       <c r="L2" s="2" t="s">
@@ -1595,46 +1580,46 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C3" t="s">
+        <v>312</v>
+      </c>
+      <c r="D3" t="s">
+        <v>316</v>
+      </c>
+      <c r="E3" t="s">
         <v>311</v>
       </c>
-      <c r="C3" t="s">
-        <v>311</v>
-      </c>
-      <c r="D3" t="s">
-        <v>312</v>
-      </c>
-      <c r="E3" t="s">
-        <v>313</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="I3" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>sub_cluster651</v>
+        <v>sub_cluster650</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>319</v>
+        <v>198</v>
       </c>
       <c r="K3" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>stg_cluster651</v>
+        <v>stg_cluster650</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>294</v>
+        <v>268</v>
       </c>
       <c r="M3" s="2"/>
       <c r="N3" s="2">
-        <v>16384</v>
+        <v>2048</v>
       </c>
       <c r="O3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P3">
         <v>1</v>
@@ -1643,82 +1628,36 @@
         <v>100</v>
       </c>
       <c r="R3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="S3">
         <v>24</v>
       </c>
       <c r="T3" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>51</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" t="s">
-        <v>317</v>
-      </c>
-      <c r="C4" t="s">
-        <v>317</v>
-      </c>
-      <c r="D4" t="s">
-        <v>321</v>
-      </c>
-      <c r="E4" t="s">
-        <v>316</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
       <c r="I4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>sub_cluster651</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>214</v>
-      </c>
+        <v>sub_</v>
+      </c>
+      <c r="J4" s="3"/>
       <c r="K4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>stg_cluster651</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>294</v>
-      </c>
+        <v>stg_</v>
+      </c>
+      <c r="L4" s="2"/>
       <c r="M4" s="2"/>
-      <c r="N4" s="2">
-        <v>2048</v>
-      </c>
-      <c r="O4">
-        <v>1</v>
-      </c>
-      <c r="P4">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>100</v>
-      </c>
-      <c r="R4" t="s">
-        <v>318</v>
-      </c>
-      <c r="S4">
-        <v>24</v>
-      </c>
-      <c r="T4" t="s">
-        <v>309</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>19</v>
-      </c>
+      <c r="N4" s="2"/>
+      <c r="U4" s="2"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
@@ -2220,7 +2159,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I31:I47" si="2">"sub_"&amp;G31</f>
         <v>sub_</v>
       </c>
       <c r="J31" s="3"/>
@@ -2239,7 +2178,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2" t="str">
-        <f t="shared" ref="I32:I48" si="2">"sub_"&amp;G32</f>
+        <f t="shared" si="2"/>
         <v>sub_</v>
       </c>
       <c r="J32" s="3"/>
@@ -2519,7 +2458,6 @@
       <c r="U46" s="2"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A47" s="2"/>
       <c r="F47" s="2"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
@@ -2538,44 +2476,26 @@
       <c r="U47" s="2"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F48" s="2"/>
-      <c r="G48" s="2"/>
       <c r="H48" s="2"/>
-      <c r="I48" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>sub_</v>
-      </c>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>stg_</v>
-      </c>
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
-      <c r="U48" s="2"/>
-    </row>
-    <row r="49" spans="8:13" x14ac:dyDescent="0.25">
-      <c r="H49" s="2"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H49" xr:uid="{4FC890E6-2DB1-4941-8EA7-F50728DEEB5D}">
-      <formula1>INDIRECT(G49)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H48" xr:uid="{4FC890E6-2DB1-4941-8EA7-F50728DEEB5D}">
+      <formula1>INDIRECT(G48)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L49:M49" xr:uid="{2D64116A-73B2-41C7-A2E1-A7FD48DA87D6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L48:M48" xr:uid="{2D64116A-73B2-41C7-A2E1-A7FD48DA87D6}">
       <formula1>INDIRECT(#REF!)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M30:M48 G2:H48 L2:L48" xr:uid="{B9C7A583-D0BF-41C2-B68D-063D33DBD67E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M29:M47 L2:L47 G2:H47" xr:uid="{B9C7A583-D0BF-41C2-B68D-063D33DBD67E}">
       <formula1>INDIRECT(SUBSTITUTE(F2,"-","_"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F48" xr:uid="{CA05F912-8685-415C-B77F-A3ADBAED34E5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F47" xr:uid="{CA05F912-8685-415C-B77F-A3ADBAED34E5}">
       <formula1>INDIRECT(A2)</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J2:J48" xr:uid="{E5C65068-C598-4D35-AC9D-0083FECA8139}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J2:J47" xr:uid="{E5C65068-C598-4D35-AC9D-0083FECA8139}">
       <formula1>INDIRECT(SUBSTITUTE(I2,"-","_"))</formula1>
     </dataValidation>
   </dataValidations>
@@ -2588,13 +2508,13 @@
           <x14:formula1>
             <xm:f>params!$B$3:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A47</xm:sqref>
+          <xm:sqref>A2:A46</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D0B35C17-C684-46B2-AA38-9FA5534C30BF}">
           <x14:formula1>
             <xm:f>params!$C$3:$C$5</xm:f>
           </x14:formula1>
-          <xm:sqref>U2:U48</xm:sqref>
+          <xm:sqref>U2:U47</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2899,13 +2819,13 @@
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C29" t="s">
         <v>232</v>
       </c>
       <c r="D29" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="E29" t="s">
         <v>249</v>

</xml_diff>

<commit_message>
SR prov gitlab-runner vm
</commit_message>
<xml_diff>
--- a/vmdefs.xlsx
+++ b/vmdefs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\My Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BF2FCFE-9023-4915-BE11-268718E90BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1A9D42-7F00-47EA-8A1D-7ECD27D3BDC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{34D50B9A-C40D-4772-AE96-867572325A1F}"/>
   </bookViews>
@@ -51,14 +51,14 @@
     <definedName name="sub_cluster481">params!$E$25:$E$41</definedName>
     <definedName name="sub_cluster650">params!$B$25:$B$41</definedName>
     <definedName name="sub_cluster651">params!$D$25:$D$41</definedName>
-    <definedName name="sub_nut_dmz_01">params!$B$69:$B$171</definedName>
-    <definedName name="sub_nut_dmz_02">params!$C$69:$C$171</definedName>
-    <definedName name="sub_nut_dmz_03">params!$D$69:$D$171</definedName>
-    <definedName name="sub_nut_dmz_04">params!$E$69:$E$171</definedName>
-    <definedName name="sub_nut_dmz_05">params!$F$69:$F$171</definedName>
-    <definedName name="sub_nut_dmz_06">params!$G$69:$G$171</definedName>
-    <definedName name="sub_nut_dmz_07">params!$H$69:$H$171</definedName>
-    <definedName name="sub_nut_dmz_08">params!$I$69:$I$171</definedName>
+    <definedName name="sub_nut_dmz_01">params!$B$69:$B$172</definedName>
+    <definedName name="sub_nut_dmz_02">params!$C$69:$C$172</definedName>
+    <definedName name="sub_nut_dmz_03">params!$D$69:$D$172</definedName>
+    <definedName name="sub_nut_dmz_04">params!$E$69:$E$172</definedName>
+    <definedName name="sub_nut_dmz_05">params!$F$69:$F$172</definedName>
+    <definedName name="sub_nut_dmz_06">params!$G$69:$G$172</definedName>
+    <definedName name="sub_nut_dmz_07">params!$H$69:$H$172</definedName>
+    <definedName name="sub_nut_dmz_08">params!$I$69:$I$172</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1147" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="315">
   <si>
     <t>DOMAIN</t>
   </si>
@@ -999,25 +999,31 @@
     <t>MEM(MB)</t>
   </si>
   <si>
-    <t>200.1.1.240</t>
-  </si>
-  <si>
-    <t>lu717</t>
-  </si>
-  <si>
-    <t>LU717</t>
-  </si>
-  <si>
-    <t>200.1.1.106</t>
-  </si>
-  <si>
     <t>var.ahv_651_network["New_PROD 192.168.25.x"]</t>
   </si>
   <si>
     <t>var.ahv_650_network["New_PROD 192.168.25.x"]</t>
   </si>
   <si>
-    <t>VM TEST LINUX -- MK417 --</t>
+    <t>PRO_DEPLOY_APP</t>
+  </si>
+  <si>
+    <t>vsl-pro-git-001</t>
+  </si>
+  <si>
+    <t>VSL-PRO-GIT-001</t>
+  </si>
+  <si>
+    <t>VSL-PRO-GIT-002</t>
+  </si>
+  <si>
+    <t>SERVEUR GITLAB RUNNER</t>
+  </si>
+  <si>
+    <t>172.23.45.1</t>
+  </si>
+  <si>
+    <t>172.23.45.254</t>
   </si>
 </sst>
 </file>
@@ -1403,10 +1409,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91DAEDD9-6941-4909-B148-BE39F1BC44CD}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:U47"/>
+  <dimension ref="A1:U46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1500,49 +1506,49 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="C2" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="D2" t="s">
         <v>312</v>
       </c>
       <c r="E2" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>36</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>12</v>
+        <v>55</v>
       </c>
       <c r="I2" s="2" t="str">
-        <f t="shared" ref="I2:I29" si="0">"sub_"&amp;G2</f>
-        <v>sub_cluster650</v>
+        <f t="shared" ref="I2:I28" si="0">"sub_"&amp;G2</f>
+        <v>sub_nut-dmz-03</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>198</v>
+        <v>308</v>
       </c>
       <c r="K2" s="3" t="str">
-        <f t="shared" ref="K2:K46" si="1">"stg_"&amp;G2</f>
-        <v>stg_cluster650</v>
+        <f t="shared" ref="K2:K45" si="1">"stg_"&amp;G2</f>
+        <v>stg_nut-dmz-03</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>268</v>
+        <v>63</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2">
-        <v>2048</v>
+        <v>16384</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P2">
         <v>1</v>
@@ -1551,16 +1557,16 @@
         <v>100</v>
       </c>
       <c r="R2" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="S2">
         <v>24</v>
       </c>
       <c r="T2" t="s">
-        <v>306</v>
+        <v>314</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -2063,7 +2069,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I29:I45" si="2">"sub_"&amp;G29</f>
         <v>sub_</v>
       </c>
       <c r="J29" s="3"/>
@@ -2082,7 +2088,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2" t="str">
-        <f t="shared" ref="I30:I46" si="2">"sub_"&amp;G30</f>
+        <f t="shared" si="2"/>
         <v>sub_</v>
       </c>
       <c r="J30" s="3"/>
@@ -2362,7 +2368,6 @@
       <c r="U44" s="2"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A45" s="2"/>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
@@ -2381,44 +2386,26 @@
       <c r="U45" s="2"/>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F46" s="2"/>
-      <c r="G46" s="2"/>
       <c r="H46" s="2"/>
-      <c r="I46" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>sub_</v>
-      </c>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>stg_</v>
-      </c>
       <c r="L46" s="2"/>
       <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
-      <c r="U46" s="2"/>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="H47" s="2"/>
-      <c r="L47" s="2"/>
-      <c r="M47" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H47" xr:uid="{4FC890E6-2DB1-4941-8EA7-F50728DEEB5D}">
-      <formula1>INDIRECT(G47)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H46" xr:uid="{4FC890E6-2DB1-4941-8EA7-F50728DEEB5D}">
+      <formula1>INDIRECT(G46)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L47:M47" xr:uid="{2D64116A-73B2-41C7-A2E1-A7FD48DA87D6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L46:M46" xr:uid="{2D64116A-73B2-41C7-A2E1-A7FD48DA87D6}">
       <formula1>INDIRECT(#REF!)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M28:M46 G2:H46 L2:L46" xr:uid="{B9C7A583-D0BF-41C2-B68D-063D33DBD67E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M27:M45 L2:L45 G2:H45" xr:uid="{B9C7A583-D0BF-41C2-B68D-063D33DBD67E}">
       <formula1>INDIRECT(SUBSTITUTE(F2,"-","_"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F46" xr:uid="{CA05F912-8685-415C-B77F-A3ADBAED34E5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F45" xr:uid="{CA05F912-8685-415C-B77F-A3ADBAED34E5}">
       <formula1>INDIRECT(A2)</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J2:J46" xr:uid="{E5C65068-C598-4D35-AC9D-0083FECA8139}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J2:J45" xr:uid="{E5C65068-C598-4D35-AC9D-0083FECA8139}">
       <formula1>INDIRECT(SUBSTITUTE(I2,"-","_"))</formula1>
     </dataValidation>
   </dataValidations>
@@ -2431,13 +2418,13 @@
           <x14:formula1>
             <xm:f>params!$B$3:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A45</xm:sqref>
+          <xm:sqref>A2:A44</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D0B35C17-C684-46B2-AA38-9FA5534C30BF}">
           <x14:formula1>
             <xm:f>params!$C$3:$C$5</xm:f>
           </x14:formula1>
-          <xm:sqref>U2:U46</xm:sqref>
+          <xm:sqref>U2:U45</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2448,10 +2435,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D40802AC-BF16-4F74-A64C-0EB8273AF630}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B2:O171"/>
+  <dimension ref="B2:O172"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView topLeftCell="C69" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68:B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2742,13 +2729,13 @@
     </row>
     <row r="29" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C29" t="s">
         <v>232</v>
       </c>
       <c r="D29" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="E29" t="s">
         <v>249</v>
@@ -6136,6 +6123,32 @@
       </c>
       <c r="I171" t="s">
         <v>195</v>
+      </c>
+    </row>
+    <row r="172" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B172" t="s">
+        <v>308</v>
+      </c>
+      <c r="C172" t="s">
+        <v>308</v>
+      </c>
+      <c r="D172" t="s">
+        <v>308</v>
+      </c>
+      <c r="E172" t="s">
+        <v>308</v>
+      </c>
+      <c r="F172" t="s">
+        <v>308</v>
+      </c>
+      <c r="G172" t="s">
+        <v>308</v>
+      </c>
+      <c r="H172" t="s">
+        <v>308</v>
+      </c>
+      <c r="I172" t="s">
+        <v>308</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test creation nouvelle vm de prepro
</commit_message>
<xml_diff>
--- a/vmdefs.xlsx
+++ b/vmdefs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\My Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE1A9D42-7F00-47EA-8A1D-7ECD27D3BDC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A1935AD-245A-420D-93DD-D85BF924B6DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{34D50B9A-C40D-4772-AE96-867572325A1F}"/>
   </bookViews>
@@ -51,14 +51,14 @@
     <definedName name="sub_cluster481">params!$E$25:$E$41</definedName>
     <definedName name="sub_cluster650">params!$B$25:$B$41</definedName>
     <definedName name="sub_cluster651">params!$D$25:$D$41</definedName>
-    <definedName name="sub_nut_dmz_01">params!$B$69:$B$172</definedName>
-    <definedName name="sub_nut_dmz_02">params!$C$69:$C$172</definedName>
-    <definedName name="sub_nut_dmz_03">params!$D$69:$D$172</definedName>
-    <definedName name="sub_nut_dmz_04">params!$E$69:$E$172</definedName>
-    <definedName name="sub_nut_dmz_05">params!$F$69:$F$172</definedName>
-    <definedName name="sub_nut_dmz_06">params!$G$69:$G$172</definedName>
-    <definedName name="sub_nut_dmz_07">params!$H$69:$H$172</definedName>
-    <definedName name="sub_nut_dmz_08">params!$I$69:$I$172</definedName>
+    <definedName name="sub_nut_dmz_01">params!$B$69:$B$184</definedName>
+    <definedName name="sub_nut_dmz_02">params!$C$69:$C$184</definedName>
+    <definedName name="sub_nut_dmz_03">params!$D$69:$D$184</definedName>
+    <definedName name="sub_nut_dmz_04">params!$E$69:$E$184</definedName>
+    <definedName name="sub_nut_dmz_05">params!$F$69:$F$184</definedName>
+    <definedName name="sub_nut_dmz_06">params!$G$69:$G$184</definedName>
+    <definedName name="sub_nut_dmz_07">params!$H$69:$H$184</definedName>
+    <definedName name="sub_nut_dmz_08">params!$I$69:$I$184</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="326">
   <si>
     <t>DOMAIN</t>
   </si>
@@ -1008,29 +1008,65 @@
     <t>PRO_DEPLOY_APP</t>
   </si>
   <si>
-    <t>vsl-pro-git-001</t>
-  </si>
-  <si>
-    <t>VSL-PRO-GIT-001</t>
-  </si>
-  <si>
-    <t>VSL-PRO-GIT-002</t>
-  </si>
-  <si>
-    <t>SERVEUR GITLAB RUNNER</t>
-  </si>
-  <si>
-    <t>172.23.45.1</t>
-  </si>
-  <si>
-    <t>172.23.45.254</t>
+    <t>PPR_REVERSE_PROXY_EXT</t>
+  </si>
+  <si>
+    <t>PPR_REVERSE_PROXY_INT</t>
+  </si>
+  <si>
+    <t>PPR_APPLICATIONS</t>
+  </si>
+  <si>
+    <t>PPR_SERVICES</t>
+  </si>
+  <si>
+    <t>PPR_EPTS</t>
+  </si>
+  <si>
+    <t>PPR_TECH_COMPONENTS</t>
+  </si>
+  <si>
+    <t>PPR_SERVICES_LN</t>
+  </si>
+  <si>
+    <t>PPR_APPLICATIONS_LN</t>
+  </si>
+  <si>
+    <t>PPR_SERVICES_LV</t>
+  </si>
+  <si>
+    <t>PPR_INNOVAS</t>
+  </si>
+  <si>
+    <t>PPR_SERVICES_DKV</t>
+  </si>
+  <si>
+    <t>PPR_SERVICES_APROBAT</t>
+  </si>
+  <si>
+    <t>VSL-PPR-RPE-001</t>
+  </si>
+  <si>
+    <t>Reverse Proxy externe</t>
+  </si>
+  <si>
+    <t>vsl-ppr-rpe-001</t>
+  </si>
+  <si>
+    <t>172.24.74.1</t>
+  </si>
+  <si>
+    <t>172.24.74.254</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1063,16 +1099,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor theme="5" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -1080,11 +1129,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1094,6 +1169,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1409,10 +1489,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91DAEDD9-6941-4909-B148-BE39F1BC44CD}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:U46"/>
+  <dimension ref="A1:U45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1428,8 +1508,8 @@
     <col min="9" max="9" width="17.85546875" customWidth="1"/>
     <col min="10" max="10" width="54.7109375" customWidth="1"/>
     <col min="11" max="11" width="3.5703125" customWidth="1"/>
-    <col min="12" max="12" width="46.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="46.5703125" customWidth="1"/>
+    <col min="12" max="12" width="23.5703125" customWidth="1"/>
+    <col min="13" max="13" width="32.140625" customWidth="1"/>
     <col min="14" max="14" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.140625" bestFit="1" customWidth="1"/>
@@ -1509,46 +1589,46 @@
         <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>310</v>
+        <v>321</v>
       </c>
       <c r="C2" t="s">
-        <v>311</v>
-      </c>
-      <c r="D2" t="s">
-        <v>312</v>
+        <v>321</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>322</v>
       </c>
       <c r="E2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="2" t="str">
+        <f t="shared" ref="I2:I27" si="0">"sub_"&amp;G2</f>
+        <v>sub_nut-dmz-02</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="I2" s="2" t="str">
-        <f t="shared" ref="I2:I28" si="0">"sub_"&amp;G2</f>
-        <v>sub_nut-dmz-03</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>308</v>
-      </c>
       <c r="K2" s="3" t="str">
-        <f t="shared" ref="K2:K45" si="1">"stg_"&amp;G2</f>
-        <v>stg_nut-dmz-03</v>
+        <f t="shared" ref="K2:K44" si="1">"stg_"&amp;G2</f>
+        <v>stg_nut-dmz-02</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="M2" s="2"/>
       <c r="N2" s="2">
-        <v>16384</v>
+        <v>4096</v>
       </c>
       <c r="O2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P2">
         <v>1</v>
@@ -1557,16 +1637,16 @@
         <v>100</v>
       </c>
       <c r="R2" t="s">
-        <v>313</v>
+        <v>324</v>
       </c>
       <c r="S2">
         <v>24</v>
       </c>
       <c r="T2" t="s">
-        <v>314</v>
+        <v>325</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>51</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -2050,7 +2130,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I28:I44" si="2">"sub_"&amp;G28</f>
         <v>sub_</v>
       </c>
       <c r="J28" s="3"/>
@@ -2069,7 +2149,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2" t="str">
-        <f t="shared" ref="I29:I45" si="2">"sub_"&amp;G29</f>
+        <f t="shared" si="2"/>
         <v>sub_</v>
       </c>
       <c r="J29" s="3"/>
@@ -2349,7 +2429,6 @@
       <c r="U43" s="2"/>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
       <c r="F44" s="2"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -2368,44 +2447,26 @@
       <c r="U44" s="2"/>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F45" s="2"/>
-      <c r="G45" s="2"/>
       <c r="H45" s="2"/>
-      <c r="I45" s="2" t="str">
-        <f t="shared" si="2"/>
-        <v>sub_</v>
-      </c>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>stg_</v>
-      </c>
       <c r="L45" s="2"/>
       <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
-      <c r="U45" s="2"/>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="H46" s="2"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H46" xr:uid="{4FC890E6-2DB1-4941-8EA7-F50728DEEB5D}">
-      <formula1>INDIRECT(G46)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H45" xr:uid="{4FC890E6-2DB1-4941-8EA7-F50728DEEB5D}">
+      <formula1>INDIRECT(G45)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L46:M46" xr:uid="{2D64116A-73B2-41C7-A2E1-A7FD48DA87D6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L45:M45" xr:uid="{2D64116A-73B2-41C7-A2E1-A7FD48DA87D6}">
       <formula1>INDIRECT(#REF!)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M27:M45 L2:L45 G2:H45" xr:uid="{B9C7A583-D0BF-41C2-B68D-063D33DBD67E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M26:M44 G2:H44 L2:L44" xr:uid="{B9C7A583-D0BF-41C2-B68D-063D33DBD67E}">
       <formula1>INDIRECT(SUBSTITUTE(F2,"-","_"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F45" xr:uid="{CA05F912-8685-415C-B77F-A3ADBAED34E5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F44" xr:uid="{CA05F912-8685-415C-B77F-A3ADBAED34E5}">
       <formula1>INDIRECT(A2)</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J2:J45" xr:uid="{E5C65068-C598-4D35-AC9D-0083FECA8139}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J2:J44" xr:uid="{E5C65068-C598-4D35-AC9D-0083FECA8139}">
       <formula1>INDIRECT(SUBSTITUTE(I2,"-","_"))</formula1>
     </dataValidation>
   </dataValidations>
@@ -2418,13 +2479,13 @@
           <x14:formula1>
             <xm:f>params!$B$3:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A44</xm:sqref>
+          <xm:sqref>A2:A43</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D0B35C17-C684-46B2-AA38-9FA5534C30BF}">
           <x14:formula1>
             <xm:f>params!$C$3:$C$5</xm:f>
           </x14:formula1>
-          <xm:sqref>U2:U45</xm:sqref>
+          <xm:sqref>U2:U44</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2435,10 +2496,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D40802AC-BF16-4F74-A64C-0EB8273AF630}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="B2:O172"/>
+  <dimension ref="B2:O184"/>
   <sheetViews>
-    <sheetView topLeftCell="C69" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68:B95"/>
+    <sheetView topLeftCell="C141" workbookViewId="0">
+      <selection activeCell="D190" sqref="D190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6151,6 +6212,318 @@
         <v>308</v>
       </c>
     </row>
+    <row r="173" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B173" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="C173" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="D173" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="E173" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="F173" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="G173" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="H173" s="5" t="s">
+        <v>309</v>
+      </c>
+      <c r="I173" s="5" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="174" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B174" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="C174" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="D174" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="E174" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="F174" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="G174" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="H174" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="I174" s="6" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="175" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B175" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="C175" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="D175" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="E175" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="F175" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="G175" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="H175" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="I175" s="5" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="176" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B176" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="C176" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="D176" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="E176" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="F176" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="G176" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="H176" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="I176" s="6" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="177" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B177" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="C177" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="D177" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="E177" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="F177" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="G177" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="H177" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="I177" s="6" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="178" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B178" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="C178" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="D178" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="E178" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="F178" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="G178" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="H178" s="5" t="s">
+        <v>314</v>
+      </c>
+      <c r="I178" s="5" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="179" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B179" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="C179" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="D179" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="E179" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="F179" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="G179" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="H179" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="I179" s="5" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="180" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B180" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="C180" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="D180" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="E180" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="F180" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="G180" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="H180" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="I180" s="6" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="181" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B181" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="C181" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="D181" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="E181" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="F181" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="G181" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="H181" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="I181" s="6" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="182" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B182" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="C182" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="D182" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="E182" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="F182" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="G182" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="H182" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="I182" s="7" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="183" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B183" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="C183" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="D183" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="E183" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="F183" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="G183" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="H183" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="I183" s="6" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="184" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B184" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="C184" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="D184" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="E184" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="F184" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="G184" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="H184" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="I184" s="8" t="s">
+        <v>320</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="B67:I67"/>

</xml_diff>

<commit_message>
test creation 6 vms prepro dmz
</commit_message>
<xml_diff>
--- a/vmdefs.xlsx
+++ b/vmdefs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\My Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716199BC-0724-436A-966C-BF479E3B4B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883F57A9-DB98-444D-8EC9-F1681359091D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{34D50B9A-C40D-4772-AE96-867572325A1F}"/>
   </bookViews>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="356">
   <si>
     <t>DOMAIN</t>
   </si>
@@ -1057,6 +1057,96 @@
   </si>
   <si>
     <t>Reverse Proxy Externe</t>
+  </si>
+  <si>
+    <t>Reverse Proxy Interne</t>
+  </si>
+  <si>
+    <t>vsl-ppr-rpi-001</t>
+  </si>
+  <si>
+    <t>VSL-PPR-RPI-001</t>
+  </si>
+  <si>
+    <t>172.24.41.1</t>
+  </si>
+  <si>
+    <t>172.24.41.254</t>
+  </si>
+  <si>
+    <t>/DMZ/Pre Prod</t>
+  </si>
+  <si>
+    <t>VSL-PPR-ALT-001</t>
+  </si>
+  <si>
+    <t>Applications  Linux</t>
+  </si>
+  <si>
+    <t>vsl-ppr-alt-001</t>
+  </si>
+  <si>
+    <t>172.24.5.1</t>
+  </si>
+  <si>
+    <t>172.24.5.254</t>
+  </si>
+  <si>
+    <t>VSL-PPR-APT-001</t>
+  </si>
+  <si>
+    <t>API Business Quarkus</t>
+  </si>
+  <si>
+    <t>vsl-ppr-apt-001</t>
+  </si>
+  <si>
+    <t>172.24.0.1</t>
+  </si>
+  <si>
+    <t>172.24.0.254</t>
+  </si>
+  <si>
+    <t>VSL-PPR-MST-001</t>
+  </si>
+  <si>
+    <t>MS Quarkus /WS springboot</t>
+  </si>
+  <si>
+    <t>vsl-ppr-mst-001</t>
+  </si>
+  <si>
+    <t>172.24.0.2</t>
+  </si>
+  <si>
+    <t>VSL-PPR-EPT-001</t>
+  </si>
+  <si>
+    <t>EPTS interne/externe</t>
+  </si>
+  <si>
+    <t>vsp-ppr-ept-001</t>
+  </si>
+  <si>
+    <t>172.24.23.1</t>
+  </si>
+  <si>
+    <t>172.24.23.254</t>
+  </si>
+  <si>
+    <t>VSL-PPR-KAF-001</t>
+  </si>
+  <si>
+    <t>KAFKA</t>
+  </si>
+  <si>
+    <t>vsl-ppr-kaf-001</t>
+  </si>
+  <si>
+    <t>172.24.11.1</t>
+  </si>
+  <si>
+    <t>172.24.11.254</t>
   </si>
 </sst>
 </file>
@@ -1121,7 +1211,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1155,11 +1245,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1173,7 +1291,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1491,8 +1616,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:U45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1594,7 +1719,7 @@
       <c r="C2" t="s">
         <v>321</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="10" t="s">
         <v>325</v>
       </c>
       <c r="E2" t="s">
@@ -1650,118 +1775,406 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
+      <c r="A3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" t="s">
+        <v>328</v>
+      </c>
+      <c r="C3" t="s">
+        <v>328</v>
+      </c>
+      <c r="D3" t="s">
+        <v>326</v>
+      </c>
+      <c r="E3" t="s">
+        <v>327</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="I3" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>sub_</v>
-      </c>
-      <c r="J3" s="3"/>
+        <v>sub_nut-dmz-04</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>310</v>
+      </c>
       <c r="K3" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>stg_</v>
-      </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="U3" s="2"/>
+        <v>stg_nut-dmz-04</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="N3" s="2">
+        <v>4096</v>
+      </c>
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>100</v>
+      </c>
+      <c r="R3" t="s">
+        <v>329</v>
+      </c>
+      <c r="S3">
+        <v>24</v>
+      </c>
+      <c r="T3" t="s">
+        <v>330</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>332</v>
+      </c>
+      <c r="C4" t="s">
+        <v>332</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>333</v>
+      </c>
+      <c r="E4" t="s">
+        <v>334</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="I4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>sub_</v>
-      </c>
-      <c r="J4" s="3"/>
+        <v>sub_nut-dmz-06</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>311</v>
+      </c>
       <c r="K4" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>stg_</v>
-      </c>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="U4" s="2"/>
+        <v>stg_nut-dmz-06</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="N4" s="2">
+        <v>4096</v>
+      </c>
+      <c r="O4">
+        <v>2</v>
+      </c>
+      <c r="P4">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>100</v>
+      </c>
+      <c r="R4" t="s">
+        <v>335</v>
+      </c>
+      <c r="S4">
+        <v>24</v>
+      </c>
+      <c r="T4" t="s">
+        <v>336</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>337</v>
+      </c>
+      <c r="C5" t="s">
+        <v>337</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>338</v>
+      </c>
+      <c r="E5" t="s">
+        <v>339</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="I5" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>sub_</v>
-      </c>
-      <c r="J5" s="3"/>
+        <v>sub_nut-dmz-08</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>312</v>
+      </c>
       <c r="K5" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>stg_</v>
-      </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="U5" s="2"/>
+        <v>stg_nut-dmz-08</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="N5" s="2">
+        <v>20480</v>
+      </c>
+      <c r="O5">
+        <v>4</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>100</v>
+      </c>
+      <c r="R5" t="s">
+        <v>340</v>
+      </c>
+      <c r="S5">
+        <v>24</v>
+      </c>
+      <c r="T5" t="s">
+        <v>341</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
+      <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>342</v>
+      </c>
+      <c r="C6" t="s">
+        <v>342</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="E6" t="s">
+        <v>344</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="I6" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>sub_</v>
-      </c>
-      <c r="J6" s="3"/>
+        <f t="shared" ref="I6" si="2">"sub_"&amp;G6</f>
+        <v>sub_nut-dmz-02</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>312</v>
+      </c>
       <c r="K6" s="3" t="str">
-        <f t="shared" si="1"/>
-        <v>stg_</v>
-      </c>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="U6" s="2"/>
+        <f t="shared" ref="K6" si="3">"stg_"&amp;G6</f>
+        <v>stg_nut-dmz-02</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="N6" s="2">
+        <v>20480</v>
+      </c>
+      <c r="O6">
+        <v>4</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="2">
+        <v>100</v>
+      </c>
+      <c r="R6" t="s">
+        <v>345</v>
+      </c>
+      <c r="S6">
+        <v>24</v>
+      </c>
+      <c r="T6" t="s">
+        <v>341</v>
+      </c>
+      <c r="U6" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="A7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>346</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>347</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>348</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="I7" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>sub_</v>
-      </c>
-      <c r="J7" s="3"/>
+        <v>sub_nut-dmz-04</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>313</v>
+      </c>
       <c r="K7" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>stg_</v>
-      </c>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="U7" s="2"/>
+        <v>stg_nut-dmz-04</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="N7" s="2">
+        <v>8192</v>
+      </c>
+      <c r="O7">
+        <v>4</v>
+      </c>
+      <c r="P7">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="2">
+        <v>100</v>
+      </c>
+      <c r="R7" t="s">
+        <v>349</v>
+      </c>
+      <c r="S7">
+        <v>24</v>
+      </c>
+      <c r="T7" t="s">
+        <v>350</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>351</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>351</v>
+      </c>
+      <c r="D8" t="s">
+        <v>352</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>353</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="I8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>sub_</v>
-      </c>
-      <c r="J8" s="3"/>
+        <v>sub_nut-dmz-06</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>314</v>
+      </c>
       <c r="K8" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>stg_</v>
-      </c>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="U8" s="2"/>
+        <v>stg_nut-dmz-06</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="N8" s="2">
+        <v>8192</v>
+      </c>
+      <c r="O8">
+        <v>4</v>
+      </c>
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="2">
+        <v>100</v>
+      </c>
+      <c r="R8" t="s">
+        <v>354</v>
+      </c>
+      <c r="S8">
+        <v>24</v>
+      </c>
+      <c r="T8" t="s">
+        <v>355</v>
+      </c>
+      <c r="U8" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
@@ -2130,7 +2543,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2" t="str">
-        <f t="shared" ref="I28:I44" si="2">"sub_"&amp;G28</f>
+        <f t="shared" ref="I28:I44" si="4">"sub_"&amp;G28</f>
         <v>sub_</v>
       </c>
       <c r="J28" s="3"/>
@@ -2149,7 +2562,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>sub_</v>
       </c>
       <c r="J29" s="3"/>
@@ -2168,7 +2581,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>sub_</v>
       </c>
       <c r="J30" s="3"/>
@@ -2187,7 +2600,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>sub_</v>
       </c>
       <c r="J31" s="3"/>
@@ -2206,7 +2619,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>sub_</v>
       </c>
       <c r="J32" s="3"/>
@@ -2225,7 +2638,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>sub_</v>
       </c>
       <c r="J33" s="3"/>
@@ -2244,7 +2657,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>sub_</v>
       </c>
       <c r="J34" s="3"/>
@@ -2263,7 +2676,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>sub_</v>
       </c>
       <c r="J35" s="3"/>
@@ -2282,7 +2695,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>sub_</v>
       </c>
       <c r="J36" s="3"/>
@@ -2301,7 +2714,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>sub_</v>
       </c>
       <c r="J37" s="3"/>
@@ -2320,7 +2733,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>sub_</v>
       </c>
       <c r="J38" s="3"/>
@@ -2339,7 +2752,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>sub_</v>
       </c>
       <c r="J39" s="3"/>
@@ -2358,7 +2771,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>sub_</v>
       </c>
       <c r="J40" s="3"/>
@@ -2377,7 +2790,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>sub_</v>
       </c>
       <c r="J41" s="3"/>
@@ -2396,7 +2809,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>sub_</v>
       </c>
       <c r="J42" s="3"/>
@@ -2415,7 +2828,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>sub_</v>
       </c>
       <c r="J43" s="3"/>
@@ -2433,7 +2846,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>sub_</v>
       </c>
       <c r="J44" s="3"/>
@@ -2460,7 +2873,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L45:M45" xr:uid="{2D64116A-73B2-41C7-A2E1-A7FD48DA87D6}">
       <formula1>INDIRECT(#REF!)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M26:M44 G2:H44 L2:L44" xr:uid="{B9C7A583-D0BF-41C2-B68D-063D33DBD67E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M26:M44 L2:L44 G2:H44" xr:uid="{B9C7A583-D0BF-41C2-B68D-063D33DBD67E}">
       <formula1>INDIRECT(SUBSTITUTE(F2,"-","_"))</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F44" xr:uid="{CA05F912-8685-415C-B77F-A3ADBAED34E5}">

</xml_diff>

<commit_message>
creation 9 autres vms prepro dmz
</commit_message>
<xml_diff>
--- a/vmdefs.xlsx
+++ b/vmdefs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\My Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883F57A9-DB98-444D-8EC9-F1681359091D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88142682-DABD-465D-8E26-A55DD4F39444}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{34D50B9A-C40D-4772-AE96-867572325A1F}"/>
   </bookViews>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1335" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1443" uniqueCount="379">
   <si>
     <t>DOMAIN</t>
   </si>
@@ -1125,9 +1125,6 @@
     <t>EPTS interne/externe</t>
   </si>
   <si>
-    <t>vsp-ppr-ept-001</t>
-  </si>
-  <si>
     <t>172.24.23.1</t>
   </si>
   <si>
@@ -1147,6 +1144,78 @@
   </si>
   <si>
     <t>172.24.11.254</t>
+  </si>
+  <si>
+    <t>VSL-PPR-ATQ-001</t>
+  </si>
+  <si>
+    <t>VSL-PPR-ATQ-002</t>
+  </si>
+  <si>
+    <t>VSL-PPR-MSN-001</t>
+  </si>
+  <si>
+    <t>VSL-PPR-ABN-001</t>
+  </si>
+  <si>
+    <t>VSL-PPR-ALN-001</t>
+  </si>
+  <si>
+    <t>VSL-PPR-ABV-001</t>
+  </si>
+  <si>
+    <t>VSL-PPR-MSV-001</t>
+  </si>
+  <si>
+    <t>VSL-PPR-ABD-001</t>
+  </si>
+  <si>
+    <t>VSL-PPR-ABA-001</t>
+  </si>
+  <si>
+    <t>172.24.1.1</t>
+  </si>
+  <si>
+    <t>172.24.1.2</t>
+  </si>
+  <si>
+    <t>172.24.1.3</t>
+  </si>
+  <si>
+    <t>172.24.1.4</t>
+  </si>
+  <si>
+    <t>172.24.6.1</t>
+  </si>
+  <si>
+    <t>172.24.2.1</t>
+  </si>
+  <si>
+    <t>172.24.2.2</t>
+  </si>
+  <si>
+    <t>172.24.3.1</t>
+  </si>
+  <si>
+    <t>172.24.4.1</t>
+  </si>
+  <si>
+    <t>172.24.1.254</t>
+  </si>
+  <si>
+    <t>172.24.6.254</t>
+  </si>
+  <si>
+    <t>172.24.2.254</t>
+  </si>
+  <si>
+    <t>172.24.3.254</t>
+  </si>
+  <si>
+    <t>172.24.4.254</t>
+  </si>
+  <si>
+    <t>vsl-ppr-ept-001</t>
   </si>
 </sst>
 </file>
@@ -1211,7 +1280,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -1273,11 +1342,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1299,6 +1396,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1617,7 +1717,7 @@
   <dimension ref="A1:U45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2056,7 +2156,7 @@
         <v>347</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>348</v>
+        <v>378</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>37</v>
@@ -2097,13 +2197,13 @@
         <v>100</v>
       </c>
       <c r="R7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="S7">
         <v>24</v>
       </c>
       <c r="T7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="U7" s="2" t="s">
         <v>19</v>
@@ -2114,16 +2214,16 @@
         <v>24</v>
       </c>
       <c r="B8" s="16" t="s">
+        <v>350</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>350</v>
+      </c>
+      <c r="D8" t="s">
         <v>351</v>
       </c>
-      <c r="C8" s="16" t="s">
-        <v>351</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" s="15" t="s">
         <v>352</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>353</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>37</v>
@@ -2164,188 +2264,602 @@
         <v>100</v>
       </c>
       <c r="R8" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="S8">
         <v>24</v>
       </c>
       <c r="T8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="U8" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="A9" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>355</v>
+      </c>
+      <c r="E9" t="str">
+        <f>LOWER(B9)</f>
+        <v>vsl-ppr-atq-001</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="I9" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>sub_</v>
-      </c>
-      <c r="J9" s="3"/>
+        <v>sub_nut-dmz-08</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>315</v>
+      </c>
       <c r="K9" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>stg_</v>
-      </c>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="U9" s="2"/>
+        <v>stg_nut-dmz-08</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="N9" s="2">
+        <v>16384</v>
+      </c>
+      <c r="O9">
+        <v>4</v>
+      </c>
+      <c r="P9">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="2">
+        <v>100</v>
+      </c>
+      <c r="R9" s="18" t="s">
+        <v>364</v>
+      </c>
+      <c r="S9">
+        <v>24</v>
+      </c>
+      <c r="T9" s="18" t="s">
+        <v>373</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>356</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>356</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" ref="E10:E17" si="4">LOWER(B10)</f>
+        <v>vsl-ppr-atq-002</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="I10" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>sub_</v>
-      </c>
-      <c r="J10" s="3"/>
+        <v>sub_nut-dmz-02</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>315</v>
+      </c>
       <c r="K10" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>stg_</v>
-      </c>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="U10" s="2"/>
+        <v>stg_nut-dmz-02</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="N10" s="2">
+        <v>8192</v>
+      </c>
+      <c r="O10">
+        <v>4</v>
+      </c>
+      <c r="P10">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>100</v>
+      </c>
+      <c r="R10" s="19" t="s">
+        <v>365</v>
+      </c>
+      <c r="S10">
+        <v>24</v>
+      </c>
+      <c r="T10" s="19" t="s">
+        <v>373</v>
+      </c>
+      <c r="U10" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
+      <c r="A11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>357</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="4"/>
+        <v>vsl-ppr-msn-001</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="I11" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>sub_</v>
-      </c>
-      <c r="J11" s="3"/>
+        <v>sub_nut-dmz-04</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>315</v>
+      </c>
       <c r="K11" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>stg_</v>
-      </c>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="U11" s="2"/>
+        <v>stg_nut-dmz-04</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="N11" s="2">
+        <v>8192</v>
+      </c>
+      <c r="O11">
+        <v>4</v>
+      </c>
+      <c r="P11">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="2">
+        <v>100</v>
+      </c>
+      <c r="R11" s="18" t="s">
+        <v>366</v>
+      </c>
+      <c r="S11">
+        <v>24</v>
+      </c>
+      <c r="T11" s="18" t="s">
+        <v>373</v>
+      </c>
+      <c r="U11" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>358</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>358</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="4"/>
+        <v>vsl-ppr-abn-001</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="I12" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>sub_</v>
-      </c>
-      <c r="J12" s="3"/>
+        <v>sub_nut-dmz-06</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>315</v>
+      </c>
       <c r="K12" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>stg_</v>
-      </c>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="U12" s="2"/>
+        <v>stg_nut-dmz-06</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="N12" s="2">
+        <v>16384</v>
+      </c>
+      <c r="O12">
+        <v>4</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>100</v>
+      </c>
+      <c r="R12" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="S12">
+        <v>24</v>
+      </c>
+      <c r="T12" s="19" t="s">
+        <v>373</v>
+      </c>
+      <c r="U12" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>359</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="4"/>
+        <v>vsl-ppr-aln-001</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="I13" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>sub_</v>
-      </c>
-      <c r="J13" s="3"/>
+        <v>sub_nut-dmz-08</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>316</v>
+      </c>
       <c r="K13" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>stg_</v>
-      </c>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="U13" s="2"/>
+        <v>stg_nut-dmz-08</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="N13" s="2">
+        <v>16384</v>
+      </c>
+      <c r="O13">
+        <v>4</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>100</v>
+      </c>
+      <c r="R13" s="18" t="s">
+        <v>368</v>
+      </c>
+      <c r="S13">
+        <v>24</v>
+      </c>
+      <c r="T13" s="18" t="s">
+        <v>374</v>
+      </c>
+      <c r="U13" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
+      <c r="A14" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>360</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="4"/>
+        <v>vsl-ppr-abv-001</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="I14" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>sub_</v>
-      </c>
-      <c r="J14" s="3"/>
+        <v>sub_nut-dmz-02</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>317</v>
+      </c>
       <c r="K14" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>stg_</v>
-      </c>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="U14" s="2"/>
+        <v>stg_nut-dmz-02</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="N14" s="2">
+        <v>4096</v>
+      </c>
+      <c r="O14">
+        <v>2</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="2">
+        <v>100</v>
+      </c>
+      <c r="R14" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="S14">
+        <v>24</v>
+      </c>
+      <c r="T14" s="19" t="s">
+        <v>375</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
+      <c r="A15" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="4"/>
+        <v>vsl-ppr-msv-001</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="I15" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>sub_</v>
-      </c>
-      <c r="J15" s="3"/>
+        <v>sub_nut-dmz-04</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>317</v>
+      </c>
       <c r="K15" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>stg_</v>
-      </c>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="U15" s="2"/>
+        <v>stg_nut-dmz-04</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="N15" s="2">
+        <v>4096</v>
+      </c>
+      <c r="O15">
+        <v>2</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="2">
+        <v>100</v>
+      </c>
+      <c r="R15" s="18" t="s">
+        <v>370</v>
+      </c>
+      <c r="S15">
+        <v>24</v>
+      </c>
+      <c r="T15" s="18" t="s">
+        <v>375</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
+      <c r="A16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>362</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>362</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="4"/>
+        <v>vsl-ppr-abd-001</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="I16" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>sub_</v>
-      </c>
-      <c r="J16" s="3"/>
+        <v>sub_nut-dmz-06</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>319</v>
+      </c>
       <c r="K16" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>stg_</v>
-      </c>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="U16" s="2"/>
+        <v>stg_nut-dmz-06</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="N16" s="2">
+        <v>8192</v>
+      </c>
+      <c r="O16">
+        <v>2</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="2">
+        <v>100</v>
+      </c>
+      <c r="R16" s="18" t="s">
+        <v>371</v>
+      </c>
+      <c r="S16">
+        <v>24</v>
+      </c>
+      <c r="T16" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="U16" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
+      <c r="A17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="17" t="s">
+        <v>363</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>363</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="4"/>
+        <v>vsl-ppr-aba-001</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>56</v>
+      </c>
       <c r="I17" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>sub_</v>
-      </c>
-      <c r="J17" s="3"/>
+        <v>sub_nut-dmz-08</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>320</v>
+      </c>
       <c r="K17" s="3" t="str">
         <f t="shared" si="1"/>
-        <v>stg_</v>
-      </c>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="U17" s="2"/>
+        <v>stg_nut-dmz-08</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="N17" s="2">
+        <v>4096</v>
+      </c>
+      <c r="O17">
+        <v>2</v>
+      </c>
+      <c r="P17">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="2">
+        <v>100</v>
+      </c>
+      <c r="R17" s="19" t="s">
+        <v>372</v>
+      </c>
+      <c r="S17">
+        <v>24</v>
+      </c>
+      <c r="T17" s="19" t="s">
+        <v>377</v>
+      </c>
+      <c r="U17" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
@@ -2543,7 +3057,7 @@
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
       <c r="I28" s="2" t="str">
-        <f t="shared" ref="I28:I44" si="4">"sub_"&amp;G28</f>
+        <f t="shared" ref="I28:I44" si="5">"sub_"&amp;G28</f>
         <v>sub_</v>
       </c>
       <c r="J28" s="3"/>
@@ -2562,7 +3076,7 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>sub_</v>
       </c>
       <c r="J29" s="3"/>
@@ -2581,7 +3095,7 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>sub_</v>
       </c>
       <c r="J30" s="3"/>
@@ -2600,7 +3114,7 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>sub_</v>
       </c>
       <c r="J31" s="3"/>
@@ -2619,7 +3133,7 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>sub_</v>
       </c>
       <c r="J32" s="3"/>
@@ -2638,7 +3152,7 @@
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>sub_</v>
       </c>
       <c r="J33" s="3"/>
@@ -2657,7 +3171,7 @@
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>sub_</v>
       </c>
       <c r="J34" s="3"/>
@@ -2676,7 +3190,7 @@
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>sub_</v>
       </c>
       <c r="J35" s="3"/>
@@ -2695,7 +3209,7 @@
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>sub_</v>
       </c>
       <c r="J36" s="3"/>
@@ -2714,7 +3228,7 @@
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>sub_</v>
       </c>
       <c r="J37" s="3"/>
@@ -2733,7 +3247,7 @@
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>sub_</v>
       </c>
       <c r="J38" s="3"/>
@@ -2752,7 +3266,7 @@
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>sub_</v>
       </c>
       <c r="J39" s="3"/>
@@ -2771,7 +3285,7 @@
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>sub_</v>
       </c>
       <c r="J40" s="3"/>
@@ -2790,7 +3304,7 @@
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>sub_</v>
       </c>
       <c r="J41" s="3"/>
@@ -2809,7 +3323,7 @@
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>sub_</v>
       </c>
       <c r="J42" s="3"/>
@@ -2828,7 +3342,7 @@
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>sub_</v>
       </c>
       <c r="J43" s="3"/>
@@ -2846,7 +3360,7 @@
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>sub_</v>
       </c>
       <c r="J44" s="3"/>
@@ -2873,7 +3387,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L45:M45" xr:uid="{2D64116A-73B2-41C7-A2E1-A7FD48DA87D6}">
       <formula1>INDIRECT(#REF!)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M26:M44 L2:L44 G2:H44" xr:uid="{B9C7A583-D0BF-41C2-B68D-063D33DBD67E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M26:M44 G2:H44 L2:L44" xr:uid="{B9C7A583-D0BF-41C2-B68D-063D33DBD67E}">
       <formula1>INDIRECT(SUBSTITUTE(F2,"-","_"))</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F44" xr:uid="{CA05F912-8685-415C-B77F-A3ADBAED34E5}">

</xml_diff>

<commit_message>
start prov 3 vm test
</commit_message>
<xml_diff>
--- a/vmdefs.xlsx
+++ b/vmdefs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\My Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1313D724-4053-495B-932A-FC756E1FF6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90B05FD-6C78-40E6-8569-F0AA0CBFE7F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{34D50B9A-C40D-4772-AE96-867572325A1F}"/>
   </bookViews>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1264" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1278" uniqueCount="334">
   <si>
     <t>DOMAIN</t>
   </si>
@@ -1066,6 +1066,21 @@
   </si>
   <si>
     <t>200.1.1.105</t>
+  </si>
+  <si>
+    <t>lu686</t>
+  </si>
+  <si>
+    <t>LU686</t>
+  </si>
+  <si>
+    <t>/DMZ/DEV</t>
+  </si>
+  <si>
+    <t>172.22.160.2</t>
+  </si>
+  <si>
+    <t>172.22.160.1</t>
   </si>
 </sst>
 </file>
@@ -1503,7 +1518,7 @@
   <dimension ref="A1:U45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1728,24 +1743,71 @@
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
+      <c r="A4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>54</v>
+      </c>
       <c r="I4" s="9" t="str">
         <f t="shared" si="0"/>
-        <v>sub_</v>
-      </c>
-      <c r="J4" s="10"/>
+        <v>sub_nut-dmz-05</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>144</v>
+      </c>
       <c r="K4" s="10" t="str">
         <f t="shared" si="1"/>
-        <v>stg_</v>
-      </c>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-      <c r="N4" s="9"/>
-      <c r="Q4" s="9"/>
-      <c r="U4" s="9"/>
+        <v>stg_nut-dmz-05</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="N4" s="9">
+        <v>1500</v>
+      </c>
+      <c r="O4" s="6">
+        <v>1</v>
+      </c>
+      <c r="P4" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="9">
+        <v>20</v>
+      </c>
+      <c r="R4" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="S4" s="6">
+        <v>24</v>
+      </c>
+      <c r="T4" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="U4" s="9" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>

</xml_diff>

<commit_message>
new VMs for Christian Kerfs
</commit_message>
<xml_diff>
--- a/vmdefs.xlsx
+++ b/vmdefs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\My Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33395170-94C3-4B26-B7AF-5679CE7B0750}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC8031D7-FB1F-4608-B208-3E052A5ADCA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{34D50B9A-C40D-4772-AE96-867572325A1F}"/>
   </bookViews>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1276" uniqueCount="331">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="334">
   <si>
     <t>DOMAIN</t>
   </si>
@@ -1056,33 +1056,31 @@
     <t>PRO_SAP_ROUTER</t>
   </si>
   <si>
-    <t>SAP ROUTER</t>
-  </si>
-  <si>
-    <r>
-      <t>VSL-PRO-SRO-001</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF353539"/>
-        <rFont val="Trebuchet MS"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-  </si>
-  <si>
-    <t>vsl-pro-sro-001</t>
-  </si>
-  <si>
-    <t>172.23.76.1</t>
-  </si>
-  <si>
-    <t>172.23.76.254</t>
-  </si>
-  <si>
     <t>PRO_SAP_ROUTER_EXT</t>
+  </si>
+  <si>
+    <t>VSL-TST-OES-001</t>
+  </si>
+  <si>
+    <t>VSL-TST-OES-002</t>
+  </si>
+  <si>
+    <t>ORACLE EXACC SCRIPT DMZ</t>
+  </si>
+  <si>
+    <t>ORACLE EXACC SCRIPT LAN</t>
+  </si>
+  <si>
+    <t>172.22.143.100</t>
+  </si>
+  <si>
+    <t>172.22.143.1</t>
+  </si>
+  <si>
+    <t>192.168.26.217</t>
+  </si>
+  <si>
+    <t>192.168.26.1</t>
   </si>
 </sst>
 </file>
@@ -1092,7 +1090,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1133,24 +1131,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF353539"/>
-      <name val="Trebuchet MS"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF353539"/>
-      <name val="Trebuchet MS"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1205,7 +1190,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1219,11 +1204,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1539,10 +1523,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91DAEDD9-6941-4909-B148-BE39F1BC44CD}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:U42"/>
+  <dimension ref="A1:U41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1555,9 +1539,9 @@
     <col min="6" max="6" width="14.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" style="6" customWidth="1"/>
-    <col min="9" max="9" width="3.85546875" style="6" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="40.140625" style="6" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" style="6" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="41.42578125" style="6" customWidth="1"/>
     <col min="13" max="13" width="22.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="10.140625" style="6" bestFit="1" customWidth="1"/>
@@ -1636,44 +1620,44 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="6" t="s">
         <v>326</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="6" t="s">
         <v>326</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F2" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="I2" s="9" t="str">
-        <f t="shared" ref="I2:I24" si="0">"sub_"&amp;G2</f>
-        <v>sub_nut-dmz-05</v>
+        <f t="shared" ref="I2:I5" si="0">"sub_"&amp;G2</f>
+        <v>sub_nut-dmz-04</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>330</v>
+        <v>95</v>
       </c>
       <c r="K2" s="10" t="str">
-        <f t="shared" ref="K2:K41" si="1">"stg_"&amp;G2</f>
-        <v>stg_nut-dmz-05</v>
+        <f t="shared" ref="K2:K40" si="1">"stg_"&amp;G2</f>
+        <v>stg_nut-dmz-04</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>323</v>
@@ -1687,45 +1671,97 @@
       <c r="P2" s="6">
         <v>1</v>
       </c>
-      <c r="Q2" s="9">
-        <v>20</v>
-      </c>
-      <c r="R2" s="12" t="s">
-        <v>328</v>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="6" t="s">
+        <v>330</v>
       </c>
       <c r="S2" s="6">
         <v>24</v>
       </c>
-      <c r="T2" s="12" t="s">
-        <v>329</v>
+      <c r="T2" s="6" t="s">
+        <v>331</v>
       </c>
       <c r="U2" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="9"/>
-      <c r="D3" s="7"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="9"/>
+      <c r="A3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>sub_cluster651</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="K3" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>stg_cluster651</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>293</v>
+      </c>
       <c r="M3" s="9"/>
-      <c r="N3" s="9"/>
+      <c r="N3" s="9">
+        <v>2048</v>
+      </c>
+      <c r="O3" s="6">
+        <v>1</v>
+      </c>
+      <c r="P3" s="6">
+        <v>1</v>
+      </c>
       <c r="Q3" s="9"/>
-      <c r="U3" s="9"/>
+      <c r="R3" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="S3" s="6">
+        <v>24</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>333</v>
+      </c>
+      <c r="U3" s="9" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="F4" s="9"/>
       <c r="G4" s="9"/>
       <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
+      <c r="I4" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>sub_</v>
+      </c>
       <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
+      <c r="K4" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>stg_</v>
+      </c>
       <c r="L4" s="9"/>
       <c r="M4" s="9"/>
       <c r="N4" s="9"/>
@@ -1737,9 +1773,15 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
+      <c r="I5" s="9" t="str">
+        <f t="shared" si="0"/>
+        <v>sub_</v>
+      </c>
       <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
+      <c r="K5" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>stg_</v>
+      </c>
       <c r="L5" s="9"/>
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
@@ -1751,9 +1793,15 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
       <c r="H6" s="9"/>
-      <c r="I6" s="9"/>
+      <c r="I6" s="9" t="str">
+        <f>"sub_"&amp;G6</f>
+        <v>sub_</v>
+      </c>
       <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
+      <c r="K6" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>stg_</v>
+      </c>
       <c r="L6" s="9"/>
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
@@ -1766,7 +1814,7 @@
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I7:I23" si="2">"sub_"&amp;G7</f>
         <v>sub_</v>
       </c>
       <c r="J7" s="10"/>
@@ -1786,7 +1834,7 @@
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>sub_</v>
       </c>
       <c r="J8" s="10"/>
@@ -1806,7 +1854,7 @@
       <c r="G9" s="9"/>
       <c r="H9" s="9"/>
       <c r="I9" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>sub_</v>
       </c>
       <c r="J9" s="10"/>
@@ -1826,7 +1874,7 @@
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>sub_</v>
       </c>
       <c r="J10" s="10"/>
@@ -1846,7 +1894,7 @@
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>sub_</v>
       </c>
       <c r="J11" s="10"/>
@@ -1866,7 +1914,7 @@
       <c r="G12" s="9"/>
       <c r="H12" s="9"/>
       <c r="I12" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>sub_</v>
       </c>
       <c r="J12" s="10"/>
@@ -1886,7 +1934,7 @@
       <c r="G13" s="9"/>
       <c r="H13" s="9"/>
       <c r="I13" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>sub_</v>
       </c>
       <c r="J13" s="10"/>
@@ -1906,7 +1954,7 @@
       <c r="G14" s="9"/>
       <c r="H14" s="9"/>
       <c r="I14" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>sub_</v>
       </c>
       <c r="J14" s="10"/>
@@ -1917,7 +1965,6 @@
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
       <c r="N14" s="9"/>
-      <c r="Q14" s="9"/>
       <c r="U14" s="9"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
@@ -1926,7 +1973,7 @@
       <c r="G15" s="9"/>
       <c r="H15" s="9"/>
       <c r="I15" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>sub_</v>
       </c>
       <c r="J15" s="10"/>
@@ -1945,7 +1992,7 @@
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>sub_</v>
       </c>
       <c r="J16" s="10"/>
@@ -1964,7 +2011,7 @@
       <c r="G17" s="9"/>
       <c r="H17" s="9"/>
       <c r="I17" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>sub_</v>
       </c>
       <c r="J17" s="10"/>
@@ -1983,7 +2030,7 @@
       <c r="G18" s="9"/>
       <c r="H18" s="9"/>
       <c r="I18" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>sub_</v>
       </c>
       <c r="J18" s="10"/>
@@ -2002,7 +2049,7 @@
       <c r="G19" s="9"/>
       <c r="H19" s="9"/>
       <c r="I19" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>sub_</v>
       </c>
       <c r="J19" s="10"/>
@@ -2021,7 +2068,7 @@
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>sub_</v>
       </c>
       <c r="J20" s="10"/>
@@ -2040,7 +2087,7 @@
       <c r="G21" s="9"/>
       <c r="H21" s="9"/>
       <c r="I21" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>sub_</v>
       </c>
       <c r="J21" s="10"/>
@@ -2059,7 +2106,7 @@
       <c r="G22" s="9"/>
       <c r="H22" s="9"/>
       <c r="I22" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>sub_</v>
       </c>
       <c r="J22" s="10"/>
@@ -2078,7 +2125,7 @@
       <c r="G23" s="9"/>
       <c r="H23" s="9"/>
       <c r="I23" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>sub_</v>
       </c>
       <c r="J23" s="10"/>
@@ -2097,7 +2144,7 @@
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="I24:I40" si="3">"sub_"&amp;G24</f>
         <v>sub_</v>
       </c>
       <c r="J24" s="10"/>
@@ -2116,7 +2163,7 @@
       <c r="G25" s="9"/>
       <c r="H25" s="9"/>
       <c r="I25" s="9" t="str">
-        <f t="shared" ref="I25:I41" si="2">"sub_"&amp;G25</f>
+        <f t="shared" si="3"/>
         <v>sub_</v>
       </c>
       <c r="J25" s="10"/>
@@ -2135,7 +2182,7 @@
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
       <c r="I26" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>sub_</v>
       </c>
       <c r="J26" s="10"/>
@@ -2154,7 +2201,7 @@
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
       <c r="I27" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>sub_</v>
       </c>
       <c r="J27" s="10"/>
@@ -2173,7 +2220,7 @@
       <c r="G28" s="9"/>
       <c r="H28" s="9"/>
       <c r="I28" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>sub_</v>
       </c>
       <c r="J28" s="10"/>
@@ -2192,7 +2239,7 @@
       <c r="G29" s="9"/>
       <c r="H29" s="9"/>
       <c r="I29" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>sub_</v>
       </c>
       <c r="J29" s="10"/>
@@ -2211,7 +2258,7 @@
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
       <c r="I30" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>sub_</v>
       </c>
       <c r="J30" s="10"/>
@@ -2230,7 +2277,7 @@
       <c r="G31" s="9"/>
       <c r="H31" s="9"/>
       <c r="I31" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>sub_</v>
       </c>
       <c r="J31" s="10"/>
@@ -2249,7 +2296,7 @@
       <c r="G32" s="9"/>
       <c r="H32" s="9"/>
       <c r="I32" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>sub_</v>
       </c>
       <c r="J32" s="10"/>
@@ -2268,7 +2315,7 @@
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
       <c r="I33" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>sub_</v>
       </c>
       <c r="J33" s="10"/>
@@ -2287,7 +2334,7 @@
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
       <c r="I34" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>sub_</v>
       </c>
       <c r="J34" s="10"/>
@@ -2306,7 +2353,7 @@
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
       <c r="I35" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>sub_</v>
       </c>
       <c r="J35" s="10"/>
@@ -2325,7 +2372,7 @@
       <c r="G36" s="9"/>
       <c r="H36" s="9"/>
       <c r="I36" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>sub_</v>
       </c>
       <c r="J36" s="10"/>
@@ -2344,7 +2391,7 @@
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
       <c r="I37" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>sub_</v>
       </c>
       <c r="J37" s="10"/>
@@ -2363,7 +2410,7 @@
       <c r="G38" s="9"/>
       <c r="H38" s="9"/>
       <c r="I38" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>sub_</v>
       </c>
       <c r="J38" s="10"/>
@@ -2382,7 +2429,7 @@
       <c r="G39" s="9"/>
       <c r="H39" s="9"/>
       <c r="I39" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>sub_</v>
       </c>
       <c r="J39" s="10"/>
@@ -2396,12 +2443,11 @@
       <c r="U39" s="9"/>
     </row>
     <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A40" s="9"/>
       <c r="F40" s="9"/>
       <c r="G40" s="9"/>
       <c r="H40" s="9"/>
       <c r="I40" s="9" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>sub_</v>
       </c>
       <c r="J40" s="10"/>
@@ -2415,44 +2461,26 @@
       <c r="U40" s="9"/>
     </row>
     <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F41" s="9"/>
-      <c r="G41" s="9"/>
       <c r="H41" s="9"/>
-      <c r="I41" s="9" t="str">
-        <f t="shared" si="2"/>
-        <v>sub_</v>
-      </c>
-      <c r="J41" s="10"/>
-      <c r="K41" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>stg_</v>
-      </c>
       <c r="L41" s="9"/>
       <c r="M41" s="9"/>
-      <c r="N41" s="9"/>
-      <c r="U41" s="9"/>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="H42" s="9"/>
-      <c r="L42" s="9"/>
-      <c r="M42" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H42" xr:uid="{4FC890E6-2DB1-4941-8EA7-F50728DEEB5D}">
-      <formula1>INDIRECT(G42)</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H41" xr:uid="{4FC890E6-2DB1-4941-8EA7-F50728DEEB5D}">
+      <formula1>INDIRECT(G41)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L42:M42" xr:uid="{2D64116A-73B2-41C7-A2E1-A7FD48DA87D6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L41:M41" xr:uid="{2D64116A-73B2-41C7-A2E1-A7FD48DA87D6}">
       <formula1>INDIRECT(#REF!)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M23:M41 L2:L41 G2:H41" xr:uid="{B9C7A583-D0BF-41C2-B68D-063D33DBD67E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M22:M40 G2:H40 L2:L40" xr:uid="{B9C7A583-D0BF-41C2-B68D-063D33DBD67E}">
       <formula1>INDIRECT(SUBSTITUTE(F2,"-","_"))</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F41" xr:uid="{CA05F912-8685-415C-B77F-A3ADBAED34E5}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F40" xr:uid="{CA05F912-8685-415C-B77F-A3ADBAED34E5}">
       <formula1>INDIRECT(A2)</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J2:J41" xr:uid="{E5C65068-C598-4D35-AC9D-0083FECA8139}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J2:J40" xr:uid="{E5C65068-C598-4D35-AC9D-0083FECA8139}">
       <formula1>INDIRECT(SUBSTITUTE(I2,"-","_"))</formula1>
     </dataValidation>
   </dataValidations>
@@ -2465,13 +2493,13 @@
           <x14:formula1>
             <xm:f>params!$B$3:$B$5</xm:f>
           </x14:formula1>
-          <xm:sqref>A2:A40</xm:sqref>
+          <xm:sqref>A2:A39</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D0B35C17-C684-46B2-AA38-9FA5534C30BF}">
           <x14:formula1>
             <xm:f>params!$C$3:$C$5</xm:f>
           </x14:formula1>
-          <xm:sqref>U2:U41</xm:sqref>
+          <xm:sqref>U2:U40</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -2484,8 +2512,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:O187"/>
   <sheetViews>
-    <sheetView topLeftCell="C147" workbookViewId="0">
-      <selection activeCell="I187" sqref="I187"/>
+    <sheetView topLeftCell="C178" workbookViewId="0">
+      <selection activeCell="D191" sqref="D191"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2504,20 +2532,20 @@
       <c r="C2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="11"/>
-      <c r="H2" s="11" t="s">
+      <c r="F2" s="12"/>
+      <c r="H2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="11"/>
-      <c r="L2" s="11" t="s">
+      <c r="I2" s="12"/>
+      <c r="L2" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
@@ -2697,12 +2725,12 @@
       </c>
     </row>
     <row r="23" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
@@ -2957,20 +2985,20 @@
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B45" s="11" t="s">
+      <c r="B45" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C45" s="11"/>
-      <c r="D45" s="11"/>
-      <c r="E45" s="11"/>
-      <c r="F45" s="11"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="11"/>
-      <c r="L45" s="11"/>
-      <c r="M45" s="11"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="12"/>
+      <c r="F45" s="12"/>
+      <c r="G45" s="12"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="12"/>
+      <c r="J45" s="12"/>
+      <c r="K45" s="12"/>
+      <c r="L45" s="12"/>
+      <c r="M45" s="12"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
@@ -3457,16 +3485,16 @@
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B67" s="11" t="s">
+      <c r="B67" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="C67" s="11"/>
-      <c r="D67" s="11"/>
-      <c r="E67" s="11"/>
-      <c r="F67" s="11"/>
-      <c r="G67" s="11"/>
-      <c r="H67" s="11"/>
-      <c r="I67" s="11"/>
+      <c r="C67" s="12"/>
+      <c r="D67" s="12"/>
+      <c r="E67" s="12"/>
+      <c r="F67" s="12"/>
+      <c r="G67" s="12"/>
+      <c r="H67" s="12"/>
+      <c r="I67" s="12"/>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
@@ -6563,29 +6591,29 @@
       </c>
     </row>
     <row r="187" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B187" s="12" t="s">
+      <c r="B187" s="11" t="s">
         <v>324</v>
       </c>
-      <c r="C187" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="D187" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="E187" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="F187" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="G187" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="H187" s="12" t="s">
-        <v>330</v>
-      </c>
-      <c r="I187" s="12" t="s">
-        <v>330</v>
+      <c r="C187" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="D187" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="E187" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="F187" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="G187" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="H187" s="11" t="s">
+        <v>325</v>
+      </c>
+      <c r="I187" s="11" t="s">
+        <v>325</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
some exa linux vms
</commit_message>
<xml_diff>
--- a/vmdefs.xlsx
+++ b/vmdefs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\My Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C3514BF-F950-44CE-BD98-E35D2D23EDFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83757A30-12F4-4981-830D-02428C49114F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{34D50B9A-C40D-4772-AE96-867572325A1F}"/>
   </bookViews>
@@ -1083,10 +1083,10 @@
     <t>192.168.26.1</t>
   </si>
   <si>
-    <t>vsl-test-oes-002</t>
-  </si>
-  <si>
-    <t>vsl-test-oes-001</t>
+    <t>vsl-tst-oes-001</t>
+  </si>
+  <si>
+    <t>vsl-tst-oes-002</t>
   </si>
 </sst>
 </file>
@@ -1532,7 +1532,7 @@
   <dimension ref="A1:U41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="W3" sqref="W3"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1640,7 +1640,7 @@
         <v>328</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F2" s="9" t="s">
         <v>36</v>
@@ -1707,7 +1707,7 @@
         <v>329</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="F3" s="9" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
ip change for vsl-pro-wik
</commit_message>
<xml_diff>
--- a/vmdefs.xlsx
+++ b/vmdefs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\My Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1FE1CE6-EC46-4CB2-BBAB-50026460A6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B081BB-BEA9-4746-B1E6-7A36A131F458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4905" yWindow="2790" windowWidth="28800" windowHeight="15435" xr2:uid="{34D50B9A-C40D-4772-AE96-867572325A1F}"/>
   </bookViews>
@@ -926,10 +926,10 @@
     <t>WIKI</t>
   </si>
   <si>
-    <t>192.168.42.165</t>
-  </si>
-  <si>
     <t>192.168.42.1</t>
+  </si>
+  <si>
+    <t>192.168.42.166</t>
   </si>
 </sst>
 </file>
@@ -1378,7 +1378,7 @@
   <dimension ref="A1:U28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="R10" sqref="R10"/>
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1590,13 +1590,13 @@
         <v>100</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="S3" s="6">
         <v>24</v>
       </c>
       <c r="T3" s="6" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="U3" s="8" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
tetsing replica IDM and replica Satellite
</commit_message>
<xml_diff>
--- a/vmdefs.xlsx
+++ b/vmdefs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\My Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D6C6F4-6D5B-4C01-AF98-C9E0D1A0F124}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2FA8174-32EB-4FE4-BB89-403CC01E37CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{34D50B9A-C40D-4772-AE96-867572325A1F}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="285">
   <si>
     <t>DOMAIN</t>
   </si>
@@ -915,6 +915,21 @@
   </si>
   <si>
     <t>192.168.25.1</t>
+  </si>
+  <si>
+    <t>RH-TESTSERVER-JH</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>rh-testserver-jh</t>
+  </si>
+  <si>
+    <t>192.168.128.98</t>
+  </si>
+  <si>
+    <t>192.168.128.1</t>
   </si>
 </sst>
 </file>
@@ -1356,7 +1371,7 @@
   <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1516,23 +1531,69 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
+      <c r="A3" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="I3" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>sub_</v>
-      </c>
-      <c r="J3" s="9"/>
+        <v>sub_pe_lu651</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>245</v>
+      </c>
       <c r="K3" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>stg_</v>
-      </c>
-      <c r="L3" s="8"/>
+        <v>stg_pe_lu651</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>233</v>
+      </c>
       <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="U3" s="8"/>
+      <c r="N3" s="8">
+        <v>2048</v>
+      </c>
+      <c r="O3" s="6">
+        <v>2</v>
+      </c>
+      <c r="P3" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="8">
+        <v>20</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="S3" s="6">
+        <v>24</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>

</xml_diff>

<commit_message>
add two new vms for axw
</commit_message>
<xml_diff>
--- a/vmdefs.xlsx
+++ b/vmdefs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\My Documents\infra\linux\prov\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9ACD9D-E796-4337-8047-8A90033AE259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CD25609-9D09-48F1-9AB6-F48B1B47BE95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{34D50B9A-C40D-4772-AE96-867572325A1F}"/>
   </bookViews>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="288">
   <si>
     <t>DOMAIN</t>
   </si>
@@ -917,16 +917,28 @@
     <t>var.ahv_651_network["521-REC_ESIGN_INT"]</t>
   </si>
   <si>
-    <t>VSL-TEST</t>
-  </si>
-  <si>
-    <t>vsltest</t>
-  </si>
-  <si>
-    <t>172.25.21.2</t>
-  </si>
-  <si>
-    <t>172.25.21.254</t>
+    <t>VSL-TST-AXW-004</t>
+  </si>
+  <si>
+    <t>vsl-tst-axw-004</t>
+  </si>
+  <si>
+    <t>192.168.42.185</t>
+  </si>
+  <si>
+    <t>192.168.42.1</t>
+  </si>
+  <si>
+    <t>VSL-TST-AXW-003</t>
+  </si>
+  <si>
+    <t>vsl-tst-axw-003</t>
+  </si>
+  <si>
+    <t>172.26.83.2</t>
+  </si>
+  <si>
+    <t>172.26.83.254</t>
   </si>
 </sst>
 </file>
@@ -1382,7 +1394,7 @@
   <dimension ref="A1:U18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1505,7 +1517,7 @@
         <v>sub_pe_lu651</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>279</v>
+        <v>207</v>
       </c>
       <c r="K2" s="9" t="str">
         <f t="shared" ref="K2:K17" si="1">"stg_"&amp;G2</f>
@@ -1541,23 +1553,69 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
+      <c r="A3" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="I3" s="8" t="str">
         <f t="shared" ref="I3:I17" si="2">"sub_"&amp;G3</f>
-        <v>sub_</v>
-      </c>
-      <c r="J3" s="9"/>
+        <v>sub_nut-dmz-04</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>262</v>
+      </c>
       <c r="K3" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>stg_</v>
-      </c>
-      <c r="L3" s="8"/>
+        <v>stg_nut-dmz-04</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="U3" s="8"/>
+      <c r="N3" s="8">
+        <v>2048</v>
+      </c>
+      <c r="O3" s="6">
+        <v>1</v>
+      </c>
+      <c r="P3" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="8">
+        <v>100</v>
+      </c>
+      <c r="R3" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="S3" s="6">
+        <v>24</v>
+      </c>
+      <c r="T3" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="U3" s="8" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="8"/>

</xml_diff>

<commit_message>
new iis dev machines
</commit_message>
<xml_diff>
--- a/vmdefs.xlsx
+++ b/vmdefs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\My Documents\infra\linux\prov\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{984F1D86-5C48-43FE-AF25-8A2886D1BF3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FDFE05-A109-4D89-A8FF-502FE8249626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{34D50B9A-C40D-4772-AE96-867572325A1F}"/>
+    <workbookView xWindow="-32370" yWindow="2655" windowWidth="28800" windowHeight="15435" xr2:uid="{34D50B9A-C40D-4772-AE96-867572325A1F}"/>
   </bookViews>
   <sheets>
     <sheet name="vms" sheetId="1" r:id="rId1"/>
@@ -929,25 +929,25 @@
     <t>REC_AUTH_INT</t>
   </si>
   <si>
-    <t>VSL-PRO-KCI-001</t>
-  </si>
-  <si>
-    <t>VSL-PRO-KCI-002</t>
-  </si>
-  <si>
-    <t>vsl-pro-kci-001</t>
-  </si>
-  <si>
-    <t>vsl-pro-kci-002</t>
-  </si>
-  <si>
-    <t>172.23.42.1</t>
-  </si>
-  <si>
-    <t>172.23.42.2</t>
-  </si>
-  <si>
-    <t>172.23.42.254</t>
+    <t>vsl-dev-iis-001</t>
+  </si>
+  <si>
+    <t>vsl-dev-idb-001</t>
+  </si>
+  <si>
+    <t>VSL-DEV-IIS-001</t>
+  </si>
+  <si>
+    <t>VSL-DEV-IDB-001</t>
+  </si>
+  <si>
+    <t>172.17.20.148</t>
+  </si>
+  <si>
+    <t>172.17.20.149</t>
+  </si>
+  <si>
+    <t>172.17.20.1</t>
   </si>
 </sst>
 </file>
@@ -1081,11 +1081,11 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1404,7 +1404,7 @@
   <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+      <selection activeCell="Q3" sqref="Q3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1499,49 +1499,49 @@
     </row>
     <row r="2" spans="1:21" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>266</v>
-      </c>
-      <c r="B2" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="E2" s="13" t="s">
         <v>284</v>
       </c>
-      <c r="C2" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>286</v>
-      </c>
       <c r="F2" s="8" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>22</v>
+        <v>270</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="I2" s="8" t="str">
         <f t="shared" ref="I2:I9" si="0">"sub_"&amp;G2</f>
-        <v>sub_nut-dmz-03</v>
+        <v>sub_pe_lu651</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>281</v>
+        <v>203</v>
       </c>
       <c r="K2" s="9" t="str">
         <f t="shared" ref="K2:K9" si="1">"stg_"&amp;G2</f>
-        <v>stg_nut-dmz-03</v>
+        <v>stg_pe_lu651</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>48</v>
+        <v>235</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8">
-        <v>2048</v>
+        <v>16384</v>
       </c>
       <c r="O2" s="6">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P2" s="6">
         <v>1</v>
@@ -1559,54 +1559,54 @@
         <v>290</v>
       </c>
       <c r="U2" s="8" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>266</v>
-      </c>
-      <c r="B3" s="13" t="s">
+        <v>265</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>285</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>285</v>
-      </c>
-      <c r="E3" s="14" t="s">
-        <v>287</v>
-      </c>
       <c r="F3" s="8" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>23</v>
+        <v>270</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="I3" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>sub_nut-dmz-04</v>
+        <v>sub_pe_lu651</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>281</v>
+        <v>203</v>
       </c>
       <c r="K3" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>stg_nut-dmz-04</v>
+        <v>stg_pe_lu651</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>49</v>
+        <v>235</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8">
-        <v>2048</v>
+        <v>8192</v>
       </c>
       <c r="O3" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P3" s="6">
         <v>1</v>
@@ -1624,7 +1624,7 @@
         <v>290</v>
       </c>
       <c r="U3" s="8" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
@@ -1812,20 +1812,20 @@
       <c r="C2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="12"/>
-      <c r="H2" s="12" t="s">
+      <c r="F2" s="14"/>
+      <c r="H2" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="12"/>
-      <c r="L2" s="12" t="s">
+      <c r="I2" s="14"/>
+      <c r="L2" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
+      <c r="M2" s="14"/>
+      <c r="N2" s="14"/>
+      <c r="O2" s="14"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
@@ -2005,12 +2005,12 @@
       </c>
     </row>
     <row r="23" spans="2:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
@@ -2167,20 +2167,20 @@
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B45" s="12" t="s">
+      <c r="B45" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="12"/>
-      <c r="D45" s="12"/>
-      <c r="E45" s="12"/>
-      <c r="F45" s="12"/>
-      <c r="G45" s="12"/>
-      <c r="H45" s="12"/>
-      <c r="I45" s="12"/>
-      <c r="J45" s="12"/>
-      <c r="K45" s="12"/>
-      <c r="L45" s="12"/>
-      <c r="M45" s="12"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="14"/>
+      <c r="H45" s="14"/>
+      <c r="I45" s="14"/>
+      <c r="J45" s="14"/>
+      <c r="K45" s="14"/>
+      <c r="L45" s="14"/>
+      <c r="M45" s="14"/>
     </row>
     <row r="46" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
@@ -2625,16 +2625,16 @@
       </c>
     </row>
     <row r="67" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B67" s="12" t="s">
+      <c r="B67" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="C67" s="12"/>
-      <c r="D67" s="12"/>
-      <c r="E67" s="12"/>
-      <c r="F67" s="12"/>
-      <c r="G67" s="12"/>
-      <c r="H67" s="12"/>
-      <c r="I67" s="12"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="14"/>
+      <c r="H67" s="14"/>
+      <c r="I67" s="14"/>
     </row>
     <row r="68" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
@@ -5783,7 +5783,7 @@
       </c>
     </row>
     <row r="189" spans="2:9" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="B189" s="13" t="s">
+      <c r="B189" s="12" t="s">
         <v>280</v>
       </c>
       <c r="C189" s="11" t="s">
@@ -5838,25 +5838,25 @@
       <c r="B191" s="6" t="s">
         <v>282</v>
       </c>
-      <c r="C191" s="13" t="s">
+      <c r="C191" s="12" t="s">
         <v>280</v>
       </c>
-      <c r="D191" s="13" t="s">
+      <c r="D191" s="12" t="s">
         <v>280</v>
       </c>
-      <c r="E191" s="13" t="s">
+      <c r="E191" s="12" t="s">
         <v>280</v>
       </c>
-      <c r="F191" s="13" t="s">
+      <c r="F191" s="12" t="s">
         <v>280</v>
       </c>
-      <c r="G191" s="13" t="s">
+      <c r="G191" s="12" t="s">
         <v>280</v>
       </c>
-      <c r="H191" s="13" t="s">
+      <c r="H191" s="12" t="s">
         <v>280</v>
       </c>
-      <c r="I191" s="13" t="s">
+      <c r="I191" s="12" t="s">
         <v>280</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2 new machines AIA & 1 new test IA
</commit_message>
<xml_diff>
--- a/vmdefs.xlsx
+++ b/vmdefs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\My Documents\infra\linux\prov\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FDFE05-A109-4D89-A8FF-502FE8249626}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE6C84D-7C0A-48F9-989A-A4F8BBAC2936}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32370" yWindow="2655" windowWidth="28800" windowHeight="15435" xr2:uid="{34D50B9A-C40D-4772-AE96-867572325A1F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{34D50B9A-C40D-4772-AE96-867572325A1F}"/>
   </bookViews>
   <sheets>
     <sheet name="vms" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
     <definedName name="sub_nut_dmz_06">params!$G$69:$G$194</definedName>
     <definedName name="sub_nut_dmz_07">params!$H$69:$H$194</definedName>
     <definedName name="sub_nut_dmz_08">params!$I$69:$I$194</definedName>
-    <definedName name="sub_pe_lu650">params!$B$25:$B$41</definedName>
+    <definedName name="sub_pe_lu650">params!$B$25:$B$44</definedName>
     <definedName name="sub_pe_lu651">params!$D$25:$D$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -75,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1310" uniqueCount="299">
   <si>
     <t>DOMAIN</t>
   </si>
@@ -929,25 +929,49 @@
     <t>REC_AUTH_INT</t>
   </si>
   <si>
-    <t>vsl-dev-iis-001</t>
-  </si>
-  <si>
-    <t>vsl-dev-idb-001</t>
-  </si>
-  <si>
-    <t>VSL-DEV-IIS-001</t>
-  </si>
-  <si>
-    <t>VSL-DEV-IDB-001</t>
-  </si>
-  <si>
-    <t>172.17.20.148</t>
-  </si>
-  <si>
-    <t>172.17.20.149</t>
-  </si>
-  <si>
-    <t>172.17.20.1</t>
+    <t>var.ahv_650_network["PRO_AIA_324"]</t>
+  </si>
+  <si>
+    <t>var.ahv_650_network["REC_AIA_524"]</t>
+  </si>
+  <si>
+    <t>var.ahv_650_network["REC_IA_547"]</t>
+  </si>
+  <si>
+    <t>vsl-pro-aia-001</t>
+  </si>
+  <si>
+    <t>VSL-PRO-AIA-001</t>
+  </si>
+  <si>
+    <t>VSL-REC-AIA-001</t>
+  </si>
+  <si>
+    <t>vsl-rec-aia-001</t>
+  </si>
+  <si>
+    <t>VSL-REC-IAI-001</t>
+  </si>
+  <si>
+    <t>vsl-rec-iai-001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.23.24.1 </t>
+  </si>
+  <si>
+    <t>172.25.24.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.25.47.1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.23.24.253 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">172.25.24.253 </t>
+  </si>
+  <si>
+    <t>172.25.47.253</t>
   </si>
 </sst>
 </file>
@@ -1403,16 +1427,14 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:U10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="6" customWidth="1"/>
     <col min="2" max="2" width="30.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="27.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="6" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.7109375" style="6" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="18" style="6" customWidth="1"/>
@@ -1501,47 +1523,47 @@
       <c r="A2" s="8" t="s">
         <v>265</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>286</v>
+      <c r="B2" t="s">
+        <v>288</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>286</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>284</v>
+        <v>288</v>
+      </c>
+      <c r="E2" t="s">
+        <v>287</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="I2" s="8" t="str">
         <f t="shared" ref="I2:I9" si="0">"sub_"&amp;G2</f>
-        <v>sub_pe_lu651</v>
+        <v>sub_pe_lu650</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>203</v>
+        <v>284</v>
       </c>
       <c r="K2" s="9" t="str">
         <f t="shared" ref="K2:K9" si="1">"stg_"&amp;G2</f>
-        <v>stg_pe_lu651</v>
+        <v>stg_pe_lu650</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="M2" s="8"/>
       <c r="N2" s="8">
-        <v>16384</v>
+        <v>24576</v>
       </c>
       <c r="O2" s="6">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="P2" s="6">
         <v>1</v>
@@ -1549,14 +1571,14 @@
       <c r="Q2" s="8">
         <v>100</v>
       </c>
-      <c r="R2" s="6" t="s">
-        <v>288</v>
+      <c r="R2" t="s">
+        <v>293</v>
       </c>
       <c r="S2" s="6">
         <v>24</v>
       </c>
-      <c r="T2" s="6" t="s">
-        <v>290</v>
+      <c r="T2" t="s">
+        <v>296</v>
       </c>
       <c r="U2" s="8" t="s">
         <v>17</v>
@@ -1567,46 +1589,46 @@
         <v>265</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="I3" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>sub_pe_lu651</v>
+        <v>sub_pe_lu650</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>203</v>
+        <v>285</v>
       </c>
       <c r="K3" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>stg_pe_lu651</v>
+        <v>stg_pe_lu650</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="M3" s="8"/>
       <c r="N3" s="8">
-        <v>8192</v>
+        <v>24576</v>
       </c>
       <c r="O3" s="6">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="P3" s="6">
         <v>1</v>
@@ -1614,37 +1636,83 @@
       <c r="Q3" s="8">
         <v>100</v>
       </c>
-      <c r="R3" s="6" t="s">
-        <v>289</v>
+      <c r="R3" t="s">
+        <v>294</v>
       </c>
       <c r="S3" s="6">
         <v>24</v>
       </c>
-      <c r="T3" s="6" t="s">
-        <v>290</v>
+      <c r="T3" t="s">
+        <v>297</v>
       </c>
       <c r="U3" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
+      <c r="A4" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="I4" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>sub_</v>
-      </c>
-      <c r="J4" s="9"/>
+        <v>sub_pe_lu650</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>286</v>
+      </c>
       <c r="K4" s="9" t="str">
         <f t="shared" si="1"/>
-        <v>stg_</v>
-      </c>
-      <c r="L4" s="8"/>
+        <v>stg_pe_lu650</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>219</v>
+      </c>
       <c r="M4" s="8"/>
-      <c r="N4" s="8"/>
-      <c r="U4" s="8"/>
+      <c r="N4" s="8">
+        <v>65535</v>
+      </c>
+      <c r="O4" s="6">
+        <v>24</v>
+      </c>
+      <c r="P4" s="6">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>100</v>
+      </c>
+      <c r="R4" t="s">
+        <v>295</v>
+      </c>
+      <c r="S4" s="6">
+        <v>24</v>
+      </c>
+      <c r="T4" t="s">
+        <v>298</v>
+      </c>
+      <c r="U4" s="8" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
@@ -1792,8 +1860,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B2:O194"/>
   <sheetViews>
-    <sheetView topLeftCell="C153" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68:B192"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2157,13 +2225,24 @@
       </c>
     </row>
     <row r="42" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>284</v>
+      </c>
       <c r="D42" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="43" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B43" t="s">
+        <v>285</v>
+      </c>
       <c r="D43" t="s">
         <v>279</v>
+      </c>
+    </row>
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.25">

</xml_diff>